<commit_message>
ctr obj xl templated updated tasks/a8badea4-b2ab-45d9-a84c-92288218e80c
</commit_message>
<xml_diff>
--- a/mosgis-web/src/main/webapp/_/libs/mosgis/Шаблон файла импорта объектов управления в ДУ.xlsx
+++ b/mosgis-web/src/main/webapp/_/libs/mosgis/Шаблон файла импорта объектов управления в ДУ.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\пользователь\Desktop\мосгис\Шаблоны Регсегмента\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\пользователь\Desktop\мосгис\Шаблоны Регсегмента\Объекты управления\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025402E6-1E9A-42D7-B004-5DA94D272457}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE475A1-0306-46FC-8178-F0543F17481B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10248" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10248" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Объекты управления" sheetId="7" r:id="rId1"/>
@@ -111,7 +111,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,12 +129,6 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -191,7 +185,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -228,22 +222,13 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -254,11 +239,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FFC6EFCE"/>
-    </mruColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -535,39 +515,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46.109375" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" style="3" customWidth="1"/>
-    <col min="3" max="4" width="22.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="38.88671875" style="3" customWidth="1"/>
     <col min="5" max="5" width="25.88671875" style="2" customWidth="1"/>
     <col min="6" max="6" width="25.109375" style="5" customWidth="1"/>
     <col min="7" max="8" width="25.109375" style="9" customWidth="1"/>
     <col min="9" max="9" width="25.109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="13" t="s">
@@ -576,13 +557,13 @@
       <c r="H1" s="13"/>
       <c r="I1" s="13"/>
     </row>
-    <row r="2" spans="1:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
       <c r="G2" s="11" t="s">
         <v>10</v>
       </c>
@@ -595,13 +576,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="C1:C2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -617,9 +598,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2"/>
+      <selection pane="topRight" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,6 +677,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <stat xmlns="7473dc27-fa1a-4161-b477-297a7233b9aa" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Документ" ma:contentTypeID="0x0101009B6B523A66479A46925D27951E2EF6F9" ma:contentTypeVersion="2" ma:contentTypeDescription="Создание документа." ma:contentTypeScope="" ma:versionID="c798f8b8a66e0569e95b99f83a778cf6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7473dc27-fa1a-4161-b477-297a7233b9aa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a06ff4e673480e1f3805eb28afa95f9" ns2:_="">
     <xsd:import namespace="7473dc27-fa1a-4161-b477-297a7233b9aa"/>
@@ -826,24 +824,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <stat xmlns="7473dc27-fa1a-4161-b477-297a7233b9aa" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3609DE5C-6380-4109-BA2D-61006CE32A38}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89813F4E-61CB-4805-9BA8-2AEB881A72FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7473dc27-fa1a-4161-b477-297a7233b9aa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBBCD727-39F5-49FF-BE46-5611C1A39AC3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -859,28 +864,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3609DE5C-6380-4109-BA2D-61006CE32A38}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89813F4E-61CB-4805-9BA8-2AEB881A72FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7473dc27-fa1a-4161-b477-297a7233b9aa"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>